<commit_message>
added 4th model, home ownership data added to zipcodes csv
</commit_message>
<xml_diff>
--- a/EDA/extradata.xlsx
+++ b/EDA/extradata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanferris/Desktop/kings_county_housing/EDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CCAE1F-AF63-0E4F-8E1F-CA2F755B08C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C45298-EC6A-834A-97DF-CB021A64DF6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="460" windowWidth="29300" windowHeight="28340" xr2:uid="{36E56F85-263C-9545-87CD-1BE8DB9E3F8A}"/>
   </bookViews>
@@ -33,38 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
   <si>
     <t>Auburn</t>
   </si>
   <si>
-    <t>Federal Way</t>
-  </si>
-  <si>
     <t>Bellevue</t>
   </si>
   <si>
-    <t>zip</t>
-  </si>
-  <si>
     <t>population</t>
   </si>
   <si>
-    <t>post office</t>
-  </si>
-  <si>
-    <t>occupied housing units</t>
-  </si>
-  <si>
-    <t>median household income</t>
-  </si>
-  <si>
-    <t>median home value</t>
-  </si>
-  <si>
-    <t>Black Diamond</t>
-  </si>
-  <si>
     <t>Bothell</t>
   </si>
   <si>
@@ -77,93 +56,30 @@
     <t>Enumclaw</t>
   </si>
   <si>
-    <t xml:space="preserve">$265,100 	</t>
-  </si>
-  <si>
-    <t>Fall City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,650 	</t>
-  </si>
-  <si>
     <t>Issaquah</t>
   </si>
   <si>
-    <t xml:space="preserve">$478,800 	</t>
-  </si>
-  <si>
     <t>Kenmore</t>
   </si>
   <si>
-    <t xml:space="preserve">24,348 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$446,900 	</t>
-  </si>
-  <si>
     <t>Kent</t>
   </si>
   <si>
-    <t xml:space="preserve">13,393 	</t>
-  </si>
-  <si>
     <t xml:space="preserve">	Kirkland</t>
   </si>
   <si>
-    <t xml:space="preserve">$103,250 	</t>
-  </si>
-  <si>
     <t>Kirkland</t>
   </si>
   <si>
-    <t xml:space="preserve">$77,688 	</t>
-  </si>
-  <si>
-    <t>Maple Valley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$317,700 	</t>
-  </si>
-  <si>
     <t>Medina</t>
   </si>
   <si>
-    <t xml:space="preserve">2,971 	</t>
-  </si>
-  <si>
-    <t>Mercer Island</t>
-  </si>
-  <si>
-    <t>North Bend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,888 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41 	</t>
-  </si>
-  <si>
     <t>Redmond</t>
   </si>
   <si>
-    <t xml:space="preserve">$465,200 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,784 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,108 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21,904 	</t>
-  </si>
-  <si>
     <t>Renton</t>
   </si>
   <si>
-    <t xml:space="preserve">12,964 	</t>
-  </si>
-  <si>
     <t xml:space="preserve">	Renton</t>
   </si>
   <si>
@@ -176,93 +92,15 @@
     <t>Woodinville</t>
   </si>
   <si>
-    <t xml:space="preserve">$107,654 	</t>
-  </si>
-  <si>
     <t>Sammamish</t>
   </si>
   <si>
-    <t xml:space="preserve">$556,000 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,733 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,585 	</t>
-  </si>
-  <si>
     <t xml:space="preserve">	Seattle</t>
   </si>
   <si>
     <t>Seattle</t>
   </si>
   <si>
-    <t xml:space="preserve">$281,700 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$74,274 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$52,276 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,638 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$53,570 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$66,408 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,180 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,770 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,511 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$56,809 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,734 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$49,233 	</t>
-  </si>
-  <si>
-    <t>population density ( ppl per sq mile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seattle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$283,100 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,111 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$40,815 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$226,800 	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,584 	</t>
-  </si>
-  <si>
-    <t>total housing units</t>
-  </si>
-  <si>
-    <t>water area (sq_mile)</t>
-  </si>
-  <si>
-    <t>land area (sq_mile)</t>
-  </si>
-  <si>
     <t>7.50</t>
   </si>
   <si>
@@ -275,9 +113,6 @@
     <t>0.75</t>
   </si>
   <si>
-    <t xml:space="preserve">10,996 	</t>
-  </si>
-  <si>
     <t>4.38</t>
   </si>
   <si>
@@ -356,9 +191,6 @@
     <t>1.71</t>
   </si>
   <si>
-    <t xml:space="preserve">17,880 	</t>
-  </si>
-  <si>
     <t>9.13</t>
   </si>
   <si>
@@ -392,9 +224,6 @@
     <t>6.04</t>
   </si>
   <si>
-    <t xml:space="preserve">25,674 	</t>
-  </si>
-  <si>
     <t>20.10</t>
   </si>
   <si>
@@ -407,18 +236,12 @@
     <t>0.18</t>
   </si>
   <si>
-    <t xml:space="preserve">13,746 	</t>
-  </si>
-  <si>
     <t>7.52</t>
   </si>
   <si>
     <t>1.55</t>
   </si>
   <si>
-    <t xml:space="preserve">13,004 	</t>
-  </si>
-  <si>
     <t>19.98</t>
   </si>
   <si>
@@ -437,9 +260,6 @@
     <t>12.83</t>
   </si>
   <si>
-    <t xml:space="preserve">9,091 	</t>
-  </si>
-  <si>
     <t>18.13</t>
   </si>
   <si>
@@ -452,18 +272,12 @@
     <t>1.63</t>
   </si>
   <si>
-    <t xml:space="preserve">4,775 	</t>
-  </si>
-  <si>
     <t>17.31</t>
   </si>
   <si>
     <t>0.22</t>
   </si>
   <si>
-    <t xml:space="preserve">14,935 	</t>
-  </si>
-  <si>
     <t>44.63</t>
   </si>
   <si>
@@ -476,9 +290,6 @@
     <t>0.25</t>
   </si>
   <si>
-    <t xml:space="preserve">24,128 	</t>
-  </si>
-  <si>
     <t>4.64</t>
   </si>
   <si>
@@ -494,18 +305,12 @@
     <t>0.32</t>
   </si>
   <si>
-    <t xml:space="preserve">12,360 	</t>
-  </si>
-  <si>
     <t>2.20</t>
   </si>
   <si>
     <t>0.27</t>
   </si>
   <si>
-    <t xml:space="preserve">8,194 	</t>
-  </si>
-  <si>
     <t>7.48</t>
   </si>
   <si>
@@ -521,9 +326,6 @@
     <t>1.48</t>
   </si>
   <si>
-    <t xml:space="preserve">21,623 	</t>
-  </si>
-  <si>
     <t>6.58</t>
   </si>
   <si>
@@ -533,18 +335,12 @@
     <t>0.73</t>
   </si>
   <si>
-    <t xml:space="preserve">14,213 	</t>
-  </si>
-  <si>
     <t>3.94</t>
   </si>
   <si>
     <t>0.61</t>
   </si>
   <si>
-    <t xml:space="preserve">16,162 	</t>
-  </si>
-  <si>
     <t>6.25</t>
   </si>
   <si>
@@ -557,9 +353,6 @@
     <t>0.63</t>
   </si>
   <si>
-    <t xml:space="preserve">17,123 	</t>
-  </si>
-  <si>
     <t>2.31</t>
   </si>
   <si>
@@ -569,9 +362,6 @@
     <t>1.54</t>
   </si>
   <si>
-    <t xml:space="preserve">9,805 	</t>
-  </si>
-  <si>
     <t>3.07</t>
   </si>
   <si>
@@ -597,6 +387,93 @@
   </si>
   <si>
     <t>1.50</t>
+  </si>
+  <si>
+    <t>postoffice</t>
+  </si>
+  <si>
+    <t>FederalWay</t>
+  </si>
+  <si>
+    <t>BlackDiamond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5650	</t>
+  </si>
+  <si>
+    <t>FallCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24348	</t>
+  </si>
+  <si>
+    <t>MapleValley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2971	</t>
+  </si>
+  <si>
+    <t>MercerIsland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13888	</t>
+  </si>
+  <si>
+    <t>NorthBend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18784	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21904	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13585	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14770	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33734	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23111	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34584	</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>pop_density(ppl_per_sq_mile)</t>
+  </si>
+  <si>
+    <t>occupied_housing_units</t>
+  </si>
+  <si>
+    <t>median_household_income</t>
+  </si>
+  <si>
+    <t>median_home_value</t>
+  </si>
+  <si>
+    <t>total_housing_units</t>
+  </si>
+  <si>
+    <t>land_area(sq_mile)</t>
+  </si>
+  <si>
+    <t>water_area(sq_mile)</t>
+  </si>
+  <si>
+    <t>owned_household_with_mortgage</t>
+  </si>
+  <si>
+    <t>renter_occupied_households</t>
+  </si>
+  <si>
+    <t>houses_owned_outright</t>
   </si>
 </sst>
 </file>
@@ -972,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C178D93-4274-4C4A-91F5-45FA01F13C14}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,43 +865,52 @@
     <col min="9" max="9" width="21.83203125" style="7" customWidth="1"/>
     <col min="10" max="10" width="21.5" style="7" customWidth="1"/>
     <col min="11" max="11" width="21.83203125" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>98001</v>
       </c>
@@ -1055,10 +941,17 @@
       <c r="J2" s="7">
         <v>0.32</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="K2" s="4">
+        <v>6975</v>
+      </c>
+      <c r="L2" s="4">
+        <v>2373</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>98002</v>
       </c>
@@ -1089,9 +982,17 @@
       <c r="J3" s="7">
         <v>0.13</v>
       </c>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="K3" s="4">
+        <v>3970</v>
+      </c>
+      <c r="L3" s="4">
+        <v>6533</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>98003</v>
       </c>
@@ -1099,7 +1000,7 @@
         <v>45892</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="D4" s="4">
         <v>3800</v>
@@ -1122,10 +1023,17 @@
       <c r="J4" s="7">
         <v>0.11</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="K4" s="4">
+        <v>6313</v>
+      </c>
+      <c r="L4" s="4">
+        <v>8770</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>98004</v>
       </c>
@@ -1133,7 +1041,7 @@
         <v>29048</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4">
         <v>3977</v>
@@ -1156,10 +1064,17 @@
       <c r="J5" s="7">
         <v>1.61</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="K5" s="4">
+        <v>4536</v>
+      </c>
+      <c r="L5" s="4">
+        <v>6666</v>
+      </c>
+      <c r="M5" s="4">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>98005</v>
       </c>
@@ -1167,7 +1082,7 @@
         <v>18412</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="4">
         <v>2361</v>
@@ -1185,15 +1100,22 @@
         <v>8070</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3193</v>
+      </c>
+      <c r="L6" s="4">
+        <v>3178</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>98006</v>
       </c>
@@ -1201,7 +1123,7 @@
         <v>37798</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>3402</v>
@@ -1219,15 +1141,22 @@
         <v>13891</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="K7" s="4">
+        <v>7907</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2638</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2743</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>98007</v>
       </c>
@@ -1235,7 +1164,7 @@
         <v>25870</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
         <v>5684</v>
@@ -1249,19 +1178,26 @@
       <c r="G8" s="3">
         <v>379000</v>
       </c>
-      <c r="H8" t="s">
-        <v>80</v>
+      <c r="H8">
+        <v>10996</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2823</v>
+      </c>
+      <c r="L8" s="4">
+        <v>6327</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>98008</v>
       </c>
@@ -1269,7 +1205,7 @@
         <v>24411</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4">
         <v>4437</v>
@@ -1287,13 +1223,22 @@
         <v>9552</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="K9" s="4">
+        <v>4854</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2545</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>98010</v>
       </c>
@@ -1301,7 +1246,7 @@
         <v>5025</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="D10">
         <v>334</v>
@@ -1319,13 +1264,22 @@
         <v>2017</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1241</v>
+      </c>
+      <c r="L10">
+        <v>273</v>
+      </c>
+      <c r="M10">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>98011</v>
       </c>
@@ -1333,7 +1287,7 @@
         <v>29212</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4">
         <v>3569</v>
@@ -1351,13 +1305,22 @@
         <v>12646</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="K11" s="4">
+        <v>6430</v>
+      </c>
+      <c r="L11" s="4">
+        <v>4007</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>98014</v>
       </c>
@@ -1365,7 +1328,7 @@
         <v>6765</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>149</v>
@@ -1388,8 +1351,17 @@
       <c r="J12" s="7">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="K12" s="4">
+        <v>1706</v>
+      </c>
+      <c r="L12">
+        <v>368</v>
+      </c>
+      <c r="M12">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>98019</v>
       </c>
@@ -1397,7 +1369,7 @@
         <v>10725</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>141</v>
@@ -1415,13 +1387,22 @@
         <v>3907</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2794</v>
+      </c>
+      <c r="L13">
+        <v>446</v>
+      </c>
+      <c r="M13">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>98022</v>
       </c>
@@ -1429,7 +1410,7 @@
         <v>20987</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>52</v>
@@ -1447,13 +1428,22 @@
         <v>9179</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="K14" s="4">
+        <v>4498</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2207</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>98023</v>
       </c>
@@ -1461,7 +1451,7 @@
         <v>47510</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="D15" s="4">
         <v>4604</v>
@@ -1472,28 +1462,37 @@
       <c r="F15" s="3">
         <v>67906</v>
       </c>
-      <c r="G15" t="s">
-        <v>14</v>
+      <c r="G15">
+        <v>265100</v>
       </c>
       <c r="H15" s="4">
         <v>18026</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K15" s="4">
+        <v>9212</v>
+      </c>
+      <c r="L15" s="4">
+        <v>5885</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>98024</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="D16">
         <v>236</v>
@@ -1514,10 +1513,19 @@
         <v>23.92</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1355</v>
+      </c>
+      <c r="L16">
+        <v>330</v>
+      </c>
+      <c r="M16">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>98027</v>
       </c>
@@ -1525,7 +1533,7 @@
         <v>26141</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>469</v>
@@ -1536,8 +1544,8 @@
       <c r="F17" s="3">
         <v>100644</v>
       </c>
-      <c r="G17" t="s">
-        <v>18</v>
+      <c r="G17">
+        <v>478800</v>
       </c>
       <c r="H17" s="4">
         <v>11248</v>
@@ -1546,10 +1554,19 @@
         <v>55.79</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="K17" s="4">
+        <v>6053</v>
+      </c>
+      <c r="L17" s="4">
+        <v>2826</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>98028</v>
       </c>
@@ -1557,7 +1574,7 @@
         <v>20419</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D18" s="4">
         <v>3606</v>
@@ -1575,21 +1592,30 @@
         <v>8566</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="K18" s="4">
+        <v>4552</v>
+      </c>
+      <c r="L18" s="4">
+        <v>2104</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>98029</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D19" s="4">
         <v>2719</v>
@@ -1600,20 +1626,29 @@
       <c r="F19" s="3">
         <v>99974</v>
       </c>
-      <c r="G19" t="s">
-        <v>21</v>
+      <c r="G19">
+        <v>446900</v>
       </c>
       <c r="H19" s="4">
         <v>10222</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5913</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2668</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>98030</v>
       </c>
@@ -1621,7 +1656,7 @@
         <v>33769</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D20" s="4">
         <v>4741</v>
@@ -1639,13 +1674,22 @@
         <v>12739</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="K20" s="4">
+        <v>5039</v>
+      </c>
+      <c r="L20" s="4">
+        <v>5994</v>
+      </c>
+      <c r="M20">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>98031</v>
       </c>
@@ -1653,7 +1697,7 @@
         <v>36581</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D21" s="4">
         <v>4877</v>
@@ -1671,13 +1715,22 @@
         <v>12846</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="K21" s="4">
+        <v>6525</v>
+      </c>
+      <c r="L21" s="4">
+        <v>4260</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>98032</v>
       </c>
@@ -1685,13 +1738,13 @@
         <v>33853</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D22" s="4">
         <v>2024</v>
       </c>
-      <c r="E22" t="s">
-        <v>23</v>
+      <c r="E22">
+        <v>13393</v>
       </c>
       <c r="F22" s="3">
         <v>48853</v>
@@ -1703,13 +1756,22 @@
         <v>14451</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="K22" s="4">
+        <v>4449</v>
+      </c>
+      <c r="L22" s="4">
+        <v>7660</v>
+      </c>
+      <c r="M22" s="4">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>98033</v>
       </c>
@@ -1717,7 +1779,7 @@
         <v>34338</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D23" s="4">
         <v>3696</v>
@@ -1725,8 +1787,8 @@
       <c r="E23" s="4">
         <v>15249</v>
       </c>
-      <c r="F23" t="s">
-        <v>25</v>
+      <c r="F23">
+        <v>103250</v>
       </c>
       <c r="G23" s="3">
         <v>528300</v>
@@ -1735,13 +1797,22 @@
         <v>16615</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="K23" s="4">
+        <v>7708</v>
+      </c>
+      <c r="L23" s="4">
+        <v>5487</v>
+      </c>
+      <c r="M23" s="4">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>98034</v>
       </c>
@@ -1749,7 +1820,7 @@
         <v>40407</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D24" s="4">
         <v>4428</v>
@@ -1757,23 +1828,32 @@
       <c r="E24" s="4">
         <v>16891</v>
       </c>
-      <c r="F24" t="s">
-        <v>27</v>
+      <c r="F24">
+        <v>77688</v>
       </c>
       <c r="G24" s="3">
         <v>364900</v>
       </c>
-      <c r="H24" t="s">
-        <v>107</v>
+      <c r="H24">
+        <v>17880</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="K24" s="4">
+        <v>8562</v>
+      </c>
+      <c r="L24" s="4">
+        <v>6542</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>98038</v>
       </c>
@@ -1781,7 +1861,7 @@
         <v>31171</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="D25" s="4">
         <v>469</v>
@@ -1792,28 +1872,37 @@
       <c r="F25" s="3">
         <v>95043</v>
       </c>
-      <c r="G25" t="s">
-        <v>29</v>
+      <c r="G25">
+        <v>317700</v>
       </c>
       <c r="H25" s="4">
         <v>11387</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="K25" s="4">
+        <v>7974</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1572</v>
+      </c>
+      <c r="M25" s="4">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>98039</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D26" s="4">
         <v>2059</v>
@@ -1831,13 +1920,22 @@
         <v>1163</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="K26" s="4">
+        <v>567</v>
+      </c>
+      <c r="L26">
+        <v>116</v>
+      </c>
+      <c r="M26">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>98040</v>
       </c>
@@ -1845,7 +1943,7 @@
         <v>22699</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="D27" s="4">
         <v>3591</v>
@@ -1866,10 +1964,19 @@
         <v>6.32</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K27" s="4">
+        <v>4427</v>
+      </c>
+      <c r="L27" s="4">
+        <v>2514</v>
+      </c>
+      <c r="M27" s="4">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>98042</v>
       </c>
@@ -1877,7 +1984,7 @@
         <v>43673</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D28" s="4">
         <v>1537</v>
@@ -1895,24 +2002,33 @@
         <v>15820</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K28" s="4">
+        <v>10606</v>
+      </c>
+      <c r="L28" s="4">
+        <v>2496</v>
+      </c>
+      <c r="M28" s="4">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>98045</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" t="s">
-        <v>35</v>
+        <v>128</v>
+      </c>
+      <c r="D29">
+        <v>41</v>
       </c>
       <c r="E29" s="4">
         <v>5192</v>
@@ -1927,13 +2043,22 @@
         <v>5536</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="K29" s="4">
+        <v>3348</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1222</v>
+      </c>
+      <c r="M29">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>98052</v>
       </c>
@@ -1941,7 +2066,7 @@
         <v>58442</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D30" s="4">
         <v>2908</v>
@@ -1952,34 +2077,43 @@
       <c r="F30" s="3">
         <v>99192</v>
       </c>
-      <c r="G30" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" t="s">
-        <v>119</v>
+      <c r="G30">
+        <v>465200</v>
+      </c>
+      <c r="H30">
+        <v>25674</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K30" s="4">
+        <v>10907</v>
+      </c>
+      <c r="L30" s="4">
+        <v>10435</v>
+      </c>
+      <c r="M30" s="4">
+        <v>2666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>98053</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D31" s="4">
         <v>662</v>
       </c>
-      <c r="E31" t="s">
-        <v>39</v>
+      <c r="E31">
+        <v>7108</v>
       </c>
       <c r="F31" s="3">
         <v>116518</v>
@@ -1991,21 +2125,30 @@
         <v>7652</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="K31" s="4">
+        <v>4917</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1000</v>
+      </c>
+      <c r="M31" s="4">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>98055</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D32" s="4">
         <v>4585</v>
@@ -2026,10 +2169,19 @@
         <v>4.78</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="K32" s="4">
+        <v>3868</v>
+      </c>
+      <c r="L32" s="4">
+        <v>3952</v>
+      </c>
+      <c r="M32">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>98056</v>
       </c>
@@ -2037,13 +2189,13 @@
         <v>32489</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D33" s="4">
         <v>4323</v>
       </c>
-      <c r="E33" t="s">
-        <v>42</v>
+      <c r="E33">
+        <v>12964</v>
       </c>
       <c r="F33" s="3">
         <v>70683</v>
@@ -2051,17 +2203,26 @@
       <c r="G33" s="3">
         <v>342600</v>
       </c>
-      <c r="H33" t="s">
-        <v>124</v>
+      <c r="H33">
+        <v>13746</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="K33" s="4">
+        <v>5908</v>
+      </c>
+      <c r="L33" s="4">
+        <v>5646</v>
+      </c>
+      <c r="M33" s="4">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>98058</v>
       </c>
@@ -2069,7 +2230,7 @@
         <v>41938</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D34" s="4">
         <v>2215</v>
@@ -2090,10 +2251,19 @@
         <v>18.93</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K34" s="4">
+        <v>8929</v>
+      </c>
+      <c r="L34" s="4">
+        <v>4196</v>
+      </c>
+      <c r="M34" s="4">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>98059</v>
       </c>
@@ -2101,7 +2271,7 @@
         <v>34463</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D35" s="4">
         <v>1725</v>
@@ -2115,17 +2285,26 @@
       <c r="G35" s="3">
         <v>363500</v>
       </c>
-      <c r="H35" t="s">
-        <v>127</v>
+      <c r="H35">
+        <v>13004</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="K35" s="4">
+        <v>7739</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2720</v>
+      </c>
+      <c r="M35" s="4">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>98065</v>
       </c>
@@ -2133,7 +2312,7 @@
         <v>12699</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D36" s="4">
         <v>171</v>
@@ -2151,13 +2330,22 @@
         <v>4556</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="K36" s="4">
+        <v>3281</v>
+      </c>
+      <c r="L36">
+        <v>674</v>
+      </c>
+      <c r="M36">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>98070</v>
       </c>
@@ -2165,7 +2353,7 @@
         <v>10624</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D37" s="4">
         <v>288</v>
@@ -2183,13 +2371,22 @@
         <v>5552</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>132</v>
+        <v>73</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="K37" s="4">
+        <v>2574</v>
+      </c>
+      <c r="L37" s="4">
+        <v>1008</v>
+      </c>
+      <c r="M37" s="4">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>98072</v>
       </c>
@@ -2197,7 +2394,7 @@
         <v>22312</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D38" s="4">
         <v>1231</v>
@@ -2205,23 +2402,32 @@
       <c r="E38" s="4">
         <v>8434</v>
       </c>
-      <c r="F38" t="s">
-        <v>47</v>
+      <c r="F38">
+        <v>107654</v>
       </c>
       <c r="G38" s="3">
         <v>466100</v>
       </c>
-      <c r="H38" t="s">
-        <v>134</v>
+      <c r="H38">
+        <v>9091</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="K38" s="4">
+        <v>5339</v>
+      </c>
+      <c r="L38" s="4">
+        <v>1906</v>
+      </c>
+      <c r="M38" s="4">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>98074</v>
       </c>
@@ -2229,7 +2435,7 @@
         <v>25748</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D39" s="4">
         <v>2411</v>
@@ -2240,8 +2446,8 @@
       <c r="F39" s="3">
         <v>143686</v>
       </c>
-      <c r="G39" t="s">
-        <v>49</v>
+      <c r="G39">
+        <v>556000</v>
       </c>
       <c r="H39" s="4">
         <v>8942</v>
@@ -2250,10 +2456,19 @@
         <v>10.68</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="K39" s="4">
+        <v>6768</v>
+      </c>
+      <c r="L39">
+        <v>934</v>
+      </c>
+      <c r="M39">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>98075</v>
       </c>
@@ -2261,13 +2476,13 @@
         <v>20715</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="D40" s="4">
         <v>2185</v>
       </c>
-      <c r="E40" t="s">
-        <v>50</v>
+      <c r="E40">
+        <v>6733</v>
       </c>
       <c r="F40" s="3">
         <v>142926</v>
@@ -2279,21 +2494,30 @@
         <v>7005</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="K40" s="4">
+        <v>5041</v>
+      </c>
+      <c r="L40">
+        <v>909</v>
+      </c>
+      <c r="M40">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>98077</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D41" s="4">
         <v>785</v>
@@ -2307,17 +2531,26 @@
       <c r="G41" s="3">
         <v>570700</v>
       </c>
-      <c r="H41" t="s">
-        <v>139</v>
+      <c r="H41">
+        <v>4775</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="K41" s="4">
+        <v>3523</v>
+      </c>
+      <c r="L41">
+        <v>304</v>
+      </c>
+      <c r="M41">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>98092</v>
       </c>
@@ -2339,17 +2572,26 @@
       <c r="G42" s="3">
         <v>287600</v>
       </c>
-      <c r="H42" t="s">
-        <v>142</v>
+      <c r="H42">
+        <v>14935</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K42" s="4">
+        <v>8352</v>
+      </c>
+      <c r="L42" s="4">
+        <v>3883</v>
+      </c>
+      <c r="M42" s="4">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>98102</v>
       </c>
@@ -2357,7 +2599,7 @@
         <v>20756</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D43" s="4">
         <v>15829</v>
@@ -2375,13 +2617,22 @@
         <v>14289</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="K43" s="4">
+        <v>2931</v>
+      </c>
+      <c r="L43" s="4">
+        <v>9193</v>
+      </c>
+      <c r="M43">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>98103</v>
       </c>
@@ -2389,7 +2640,7 @@
         <v>45911</v>
       </c>
       <c r="C44" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D44" s="4">
         <v>9905</v>
@@ -2403,17 +2654,26 @@
       <c r="G44" s="3">
         <v>478200</v>
       </c>
-      <c r="H44" t="s">
-        <v>147</v>
+      <c r="H44">
+        <v>24128</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="K44" s="4">
+        <v>8672</v>
+      </c>
+      <c r="L44" s="4">
+        <v>11858</v>
+      </c>
+      <c r="M44" s="4">
+        <v>2194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>98105</v>
       </c>
@@ -2421,7 +2681,7 @@
         <v>43924</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D45" s="4">
         <v>10643</v>
@@ -2439,13 +2699,22 @@
         <v>17161</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="K45" s="4">
+        <v>4001</v>
+      </c>
+      <c r="L45" s="4">
+        <v>10435</v>
+      </c>
+      <c r="M45" s="4">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>98106</v>
       </c>
@@ -2453,7 +2722,7 @@
         <v>22873</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D46" s="4">
         <v>4161</v>
@@ -2464,20 +2733,29 @@
       <c r="F46" s="3">
         <v>57875</v>
       </c>
-      <c r="G46" t="s">
-        <v>54</v>
+      <c r="G46">
+        <v>281700</v>
       </c>
       <c r="H46" s="4">
         <v>9990</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="K46" s="4">
+        <v>4089</v>
+      </c>
+      <c r="L46" s="4">
+        <v>4132</v>
+      </c>
+      <c r="M46">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>98107</v>
       </c>
@@ -2485,7 +2763,7 @@
         <v>21147</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D47" s="4">
         <v>9602</v>
@@ -2499,17 +2777,26 @@
       <c r="G47" s="3">
         <v>447700</v>
       </c>
-      <c r="H47" t="s">
-        <v>153</v>
+      <c r="H47">
+        <v>12360</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="K47" s="4">
+        <v>3813</v>
+      </c>
+      <c r="L47" s="4">
+        <v>6575</v>
+      </c>
+      <c r="M47">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>98108</v>
       </c>
@@ -2517,7 +2804,7 @@
         <v>22374</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D48" s="4">
         <v>2989</v>
@@ -2531,17 +2818,26 @@
       <c r="G48" s="3">
         <v>326500</v>
       </c>
-      <c r="H48" t="s">
-        <v>156</v>
+      <c r="H48">
+        <v>8194</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>157</v>
+        <v>92</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="K48" s="4">
+        <v>3099</v>
+      </c>
+      <c r="L48" s="4">
+        <v>3350</v>
+      </c>
+      <c r="M48" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>98109</v>
       </c>
@@ -2549,7 +2845,7 @@
         <v>20715</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D49" s="4">
         <v>10361</v>
@@ -2567,13 +2863,22 @@
         <v>13906</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K49" s="4">
+        <v>3123</v>
+      </c>
+      <c r="L49" s="4">
+        <v>8475</v>
+      </c>
+      <c r="M49">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>98112</v>
       </c>
@@ -2581,7 +2886,7 @@
         <v>21077</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D50" s="4">
         <v>6667</v>
@@ -2602,10 +2907,19 @@
         <v>3.16</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K50" s="4">
+        <v>4045</v>
+      </c>
+      <c r="L50" s="4">
+        <v>4551</v>
+      </c>
+      <c r="M50" s="4">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>98115</v>
       </c>
@@ -2613,7 +2927,7 @@
         <v>46206</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D51" s="4">
         <v>7018</v>
@@ -2627,17 +2941,26 @@
       <c r="G51" s="3">
         <v>492700</v>
       </c>
-      <c r="H51" t="s">
-        <v>162</v>
+      <c r="H51">
+        <v>21623</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="K51" s="4">
+        <v>9646</v>
+      </c>
+      <c r="L51" s="4">
+        <v>7271</v>
+      </c>
+      <c r="M51" s="4">
+        <v>3539</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>98116</v>
       </c>
@@ -2645,7 +2968,7 @@
         <v>22241</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D52" s="4">
         <v>7523</v>
@@ -2653,8 +2976,8 @@
       <c r="E52" s="4">
         <v>11104</v>
       </c>
-      <c r="F52" t="s">
-        <v>55</v>
+      <c r="F52">
+        <v>74274</v>
       </c>
       <c r="G52" s="3">
         <v>467900</v>
@@ -2666,10 +2989,19 @@
         <v>2.96</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="K52" s="4">
+        <v>4964</v>
+      </c>
+      <c r="L52" s="4">
+        <v>4644</v>
+      </c>
+      <c r="M52" s="4">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>98117</v>
       </c>
@@ -2677,7 +3009,7 @@
         <v>31365</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D53" s="4">
         <v>7953</v>
@@ -2691,17 +3023,26 @@
       <c r="G53" s="3">
         <v>463500</v>
       </c>
-      <c r="H53" t="s">
-        <v>166</v>
+      <c r="H53">
+        <v>14213</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K53" s="4">
+        <v>7628</v>
+      </c>
+      <c r="L53" s="4">
+        <v>3779</v>
+      </c>
+      <c r="M53" s="4">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>98118</v>
       </c>
@@ -2709,7 +3050,7 @@
         <v>42731</v>
       </c>
       <c r="C54" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D54" s="4">
         <v>6841</v>
@@ -2717,23 +3058,32 @@
       <c r="E54" s="4">
         <v>15127</v>
       </c>
-      <c r="F54" t="s">
-        <v>56</v>
+      <c r="F54">
+        <v>52276</v>
       </c>
       <c r="G54" s="3">
         <v>350700</v>
       </c>
-      <c r="H54" t="s">
-        <v>169</v>
+      <c r="H54">
+        <v>16162</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>170</v>
+        <v>102</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="K54" s="4">
+        <v>7064</v>
+      </c>
+      <c r="L54" s="4">
+        <v>6266</v>
+      </c>
+      <c r="M54" s="4">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>98119</v>
       </c>
@@ -2741,10 +3091,10 @@
         <v>21039</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" t="s">
-        <v>57</v>
+        <v>21</v>
+      </c>
+      <c r="D55">
+        <v>8638</v>
       </c>
       <c r="E55" s="4">
         <v>10682</v>
@@ -2759,13 +3109,22 @@
         <v>11592</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>172</v>
+        <v>104</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="K55" s="4">
+        <v>3500</v>
+      </c>
+      <c r="L55" s="4">
+        <v>6193</v>
+      </c>
+      <c r="M55">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>98122</v>
       </c>
@@ -2773,7 +3132,7 @@
         <v>31454</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D56" s="4">
         <v>13594</v>
@@ -2781,23 +3140,32 @@
       <c r="E56" s="4">
         <v>15717</v>
       </c>
-      <c r="F56" t="s">
-        <v>58</v>
+      <c r="F56">
+        <v>53570</v>
       </c>
       <c r="G56" s="3">
         <v>407600</v>
       </c>
-      <c r="H56" t="s">
-        <v>174</v>
+      <c r="H56">
+        <v>17123</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>175</v>
+        <v>106</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="K56" s="4">
+        <v>4501</v>
+      </c>
+      <c r="L56" s="4">
+        <v>10349</v>
+      </c>
+      <c r="M56">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>98125</v>
       </c>
@@ -2805,7 +3173,7 @@
         <v>37081</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D57" s="4">
         <v>6879</v>
@@ -2826,10 +3194,19 @@
         <v>5.39</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="K57" s="4">
+        <v>6108</v>
+      </c>
+      <c r="L57" s="4">
+        <v>8962</v>
+      </c>
+      <c r="M57" s="4">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>98126</v>
       </c>
@@ -2837,7 +3214,7 @@
         <v>20698</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D58" s="4">
         <v>6732</v>
@@ -2845,23 +3222,32 @@
       <c r="E58" s="4">
         <v>9190</v>
       </c>
-      <c r="F58" t="s">
-        <v>59</v>
+      <c r="F58">
+        <v>66408</v>
       </c>
       <c r="G58" s="3">
         <v>358100</v>
       </c>
-      <c r="H58" t="s">
-        <v>178</v>
+      <c r="H58">
+        <v>9805</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="K58" s="4">
+        <v>4387</v>
+      </c>
+      <c r="L58" s="4">
+        <v>3814</v>
+      </c>
+      <c r="M58">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>98133</v>
       </c>
@@ -2869,13 +3255,13 @@
         <v>44555</v>
       </c>
       <c r="C59" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D59" s="4">
         <v>6279</v>
       </c>
-      <c r="E59" t="s">
-        <v>60</v>
+      <c r="E59">
+        <v>20180</v>
       </c>
       <c r="F59" s="3">
         <v>51499</v>
@@ -2890,18 +3276,27 @@
         <v>7.1</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="K59" s="4">
+        <v>7568</v>
+      </c>
+      <c r="L59" s="4">
+        <v>10211</v>
+      </c>
+      <c r="M59" s="4">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>98136</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D60" s="4">
         <v>6425</v>
@@ -2922,10 +3317,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="K60" s="4">
+        <v>3551</v>
+      </c>
+      <c r="L60" s="4">
+        <v>2448</v>
+      </c>
+      <c r="M60" s="4">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>98144</v>
       </c>
@@ -2933,13 +3337,13 @@
         <v>26881</v>
       </c>
       <c r="C61" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D61" s="4">
         <v>7895</v>
       </c>
-      <c r="E61" t="s">
-        <v>62</v>
+      <c r="E61">
+        <v>11511</v>
       </c>
       <c r="F61" s="3">
         <v>55950</v>
@@ -2954,10 +3358,19 @@
         <v>3.4</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="K61" s="4">
+        <v>4367</v>
+      </c>
+      <c r="L61" s="4">
+        <v>5874</v>
+      </c>
+      <c r="M61" s="4">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>98146</v>
       </c>
@@ -2965,7 +3378,7 @@
         <v>25922</v>
       </c>
       <c r="C62" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D62" s="4">
         <v>5573</v>
@@ -2973,8 +3386,8 @@
       <c r="E62" s="4">
         <v>9611</v>
       </c>
-      <c r="F62" t="s">
-        <v>63</v>
+      <c r="F62">
+        <v>56809</v>
       </c>
       <c r="G62" s="3">
         <v>308400</v>
@@ -2983,13 +3396,22 @@
         <v>10222</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="K62" s="4">
+        <v>4551</v>
+      </c>
+      <c r="L62" s="4">
+        <v>3565</v>
+      </c>
+      <c r="M62" s="4">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>98148</v>
       </c>
@@ -2997,7 +3419,7 @@
         <v>10010</v>
       </c>
       <c r="C63" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D63" s="4">
         <v>3194</v>
@@ -3020,8 +3442,17 @@
       <c r="J63" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="K63" s="4">
+        <v>1418</v>
+      </c>
+      <c r="L63" s="4">
+        <v>2411</v>
+      </c>
+      <c r="M63">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>98155</v>
       </c>
@@ -3029,7 +3460,7 @@
         <v>32778</v>
       </c>
       <c r="C64" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D64" s="4">
         <v>4330</v>
@@ -3052,8 +3483,17 @@
       <c r="J64" s="7">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="K64" s="4">
+        <v>7007</v>
+      </c>
+      <c r="L64" s="4">
+        <v>4051</v>
+      </c>
+      <c r="M64" s="4">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>98166</v>
       </c>
@@ -3061,7 +3501,7 @@
         <v>20301</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D65" s="4">
         <v>3580</v>
@@ -3084,16 +3524,25 @@
       <c r="J65" s="7">
         <v>1.56</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="K65" s="4">
+        <v>3826</v>
+      </c>
+      <c r="L65" s="4">
+        <v>2832</v>
+      </c>
+      <c r="M65" s="4">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>98168</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="C66" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D66" s="4">
         <v>3794</v>
@@ -3101,8 +3550,8 @@
       <c r="E66" s="4">
         <v>11678</v>
       </c>
-      <c r="F66" t="s">
-        <v>65</v>
+      <c r="F66">
+        <v>49233</v>
       </c>
       <c r="G66" s="3">
         <v>240000</v>
@@ -3114,10 +3563,19 @@
         <v>8.89</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="K66" s="4">
+        <v>5058</v>
+      </c>
+      <c r="L66" s="4">
+        <v>5292</v>
+      </c>
+      <c r="M66" s="4">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>98177</v>
       </c>
@@ -3125,7 +3583,7 @@
         <v>19030</v>
       </c>
       <c r="C67" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D67" s="4">
         <v>3341</v>
@@ -3148,8 +3606,17 @@
       <c r="J67" s="7">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="K67" s="4">
+        <v>4517</v>
+      </c>
+      <c r="L67" s="4">
+        <v>1350</v>
+      </c>
+      <c r="M67" s="4">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>98178</v>
       </c>
@@ -3157,7 +3624,7 @@
         <v>24092</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D68" s="4">
         <v>4966</v>
@@ -3168,8 +3635,8 @@
       <c r="F68" s="3">
         <v>58707</v>
       </c>
-      <c r="G68" t="s">
-        <v>68</v>
+      <c r="G68">
+        <v>283100</v>
       </c>
       <c r="H68" s="4">
         <v>9290</v>
@@ -3180,16 +3647,25 @@
       <c r="J68" s="7">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="K68" s="4">
+        <v>4332</v>
+      </c>
+      <c r="L68" s="4">
+        <v>2996</v>
+      </c>
+      <c r="M68" s="4">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>98188</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C69" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D69" s="4">
         <v>3062</v>
@@ -3197,11 +3673,11 @@
       <c r="E69" s="4">
         <v>9263</v>
       </c>
-      <c r="F69" t="s">
-        <v>70</v>
-      </c>
-      <c r="G69" t="s">
-        <v>71</v>
+      <c r="F69">
+        <v>40815</v>
+      </c>
+      <c r="G69">
+        <v>226800</v>
       </c>
       <c r="H69" s="4">
         <v>9959</v>
@@ -3212,16 +3688,25 @@
       <c r="J69" s="7">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="K69" s="4">
+        <v>3088</v>
+      </c>
+      <c r="L69" s="4">
+        <v>4840</v>
+      </c>
+      <c r="M69" s="4">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>98198</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="C70" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D70" s="4">
         <v>4441</v>
@@ -3244,8 +3729,17 @@
       <c r="J70" s="7">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="K70" s="4">
+        <v>5705</v>
+      </c>
+      <c r="L70" s="4">
+        <v>5602</v>
+      </c>
+      <c r="M70" s="4">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>98199</v>
       </c>
@@ -3253,7 +3747,7 @@
         <v>19686</v>
       </c>
       <c r="C71" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D71" s="4">
         <v>4714</v>
@@ -3274,7 +3768,16 @@
         <v>4.18</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>187</v>
+        <v>117</v>
+      </c>
+      <c r="K71" s="4">
+        <v>4381</v>
+      </c>
+      <c r="L71" s="4">
+        <v>3160</v>
+      </c>
+      <c r="M71" s="4">
+        <v>1557</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
additional zipcode data added
</commit_message>
<xml_diff>
--- a/EDA/extradata.xlsx
+++ b/EDA/extradata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanferris/Desktop/kings_county_housing/EDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C45298-EC6A-834A-97DF-CB021A64DF6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72192FD6-DE63-C241-8141-B32BE179319E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="460" windowWidth="29300" windowHeight="28340" xr2:uid="{36E56F85-263C-9545-87CD-1BE8DB9E3F8A}"/>
+    <workbookView xWindow="11560" yWindow="460" windowWidth="29300" windowHeight="28340" xr2:uid="{36E56F85-263C-9545-87CD-1BE8DB9E3F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
   <si>
     <t>Auburn</t>
   </si>
@@ -446,9 +446,6 @@
     <t>zipcode</t>
   </si>
   <si>
-    <t>pop_density(ppl_per_sq_mile)</t>
-  </si>
-  <si>
     <t>occupied_housing_units</t>
   </si>
   <si>
@@ -461,12 +458,6 @@
     <t>total_housing_units</t>
   </si>
   <si>
-    <t>land_area(sq_mile)</t>
-  </si>
-  <si>
-    <t>water_area(sq_mile)</t>
-  </si>
-  <si>
     <t>owned_household_with_mortgage</t>
   </si>
   <si>
@@ -474,6 +465,21 @@
   </si>
   <si>
     <t>houses_owned_outright</t>
+  </si>
+  <si>
+    <t>sold_and_unoccupied</t>
+  </si>
+  <si>
+    <t>seasonal_or_rec_use</t>
+  </si>
+  <si>
+    <t>pop_density</t>
+  </si>
+  <si>
+    <t>land_area</t>
+  </si>
+  <si>
+    <t>water_area_sq_mile</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,13 +511,38 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -526,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -535,6 +566,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C178D93-4274-4C4A-91F5-45FA01F13C14}">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,7 +903,7 @@
     <col min="13" max="13" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>136</v>
       </c>
@@ -880,38 +914,44 @@
         <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="M1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    </row>
+    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>98001</v>
       </c>
       <c r="B2">
@@ -950,9 +990,15 @@
       <c r="M2" s="4">
         <v>1369</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="N2" s="10">
+        <v>21</v>
+      </c>
+      <c r="O2" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>98002</v>
       </c>
       <c r="B3">
@@ -991,9 +1037,15 @@
       <c r="M3" s="4">
         <v>1992</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="N3" s="10">
+        <v>28</v>
+      </c>
+      <c r="O3" s="10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>98003</v>
       </c>
       <c r="B4">
@@ -1032,9 +1084,15 @@
       <c r="M4" s="4">
         <v>2167</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="N4" s="10">
+        <v>39</v>
+      </c>
+      <c r="O4" s="10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>98004</v>
       </c>
       <c r="B5">
@@ -1073,9 +1131,15 @@
       <c r="M5" s="4">
         <v>2118</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="N5" s="10">
+        <v>60</v>
+      </c>
+      <c r="O5" s="10">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>98005</v>
       </c>
       <c r="B6">
@@ -1114,9 +1178,15 @@
       <c r="M6" s="4">
         <v>1168</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="N6" s="10">
+        <v>29</v>
+      </c>
+      <c r="O6" s="10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>98006</v>
       </c>
       <c r="B7">
@@ -1155,9 +1225,15 @@
       <c r="M7" s="4">
         <v>2743</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="N7" s="10">
+        <v>38</v>
+      </c>
+      <c r="O7" s="10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>98007</v>
       </c>
       <c r="B8">
@@ -1196,9 +1272,15 @@
       <c r="M8" s="4">
         <v>1165</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="N8" s="10">
+        <v>10</v>
+      </c>
+      <c r="O8" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>98008</v>
       </c>
       <c r="B9" s="4">
@@ -1237,9 +1319,15 @@
       <c r="M9" s="4">
         <v>1774</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="N9" s="10">
+        <v>29</v>
+      </c>
+      <c r="O9" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>98010</v>
       </c>
       <c r="B10" s="4">
@@ -1278,9 +1366,15 @@
       <c r="M10">
         <v>332</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="N10" s="10">
+        <v>2</v>
+      </c>
+      <c r="O10" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>98011</v>
       </c>
       <c r="B11" s="4">
@@ -1319,9 +1413,15 @@
       <c r="M11" s="4">
         <v>1468</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="N11" s="10">
+        <v>23</v>
+      </c>
+      <c r="O11" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>98014</v>
       </c>
       <c r="B12" s="4">
@@ -1360,9 +1460,15 @@
       <c r="M12">
         <v>382</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="N12" s="10">
+        <v>5</v>
+      </c>
+      <c r="O12" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>98019</v>
       </c>
       <c r="B13" s="4">
@@ -1401,9 +1507,15 @@
       <c r="M13">
         <v>468</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="N13" s="10">
+        <v>18</v>
+      </c>
+      <c r="O13" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>98022</v>
       </c>
       <c r="B14" s="4">
@@ -1442,9 +1554,15 @@
       <c r="M14" s="4">
         <v>1591</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="N14" s="10">
+        <v>21</v>
+      </c>
+      <c r="O14" s="10">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>98023</v>
       </c>
       <c r="B15" s="4">
@@ -1483,9 +1601,15 @@
       <c r="M15" s="4">
         <v>1815</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="N15" s="10">
+        <v>46</v>
+      </c>
+      <c r="O15" s="10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>98024</v>
       </c>
       <c r="B16" t="s">
@@ -1524,9 +1648,15 @@
       <c r="M16">
         <v>394</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="N16" s="10">
+        <v>13</v>
+      </c>
+      <c r="O16" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>98027</v>
       </c>
       <c r="B17" s="4">
@@ -1565,9 +1695,15 @@
       <c r="M17" s="4">
         <v>1575</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="N17" s="10">
+        <v>45</v>
+      </c>
+      <c r="O17" s="10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <v>98028</v>
       </c>
       <c r="B18" s="4">
@@ -1606,9 +1742,15 @@
       <c r="M18" s="4">
         <v>1325</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="N18" s="10">
+        <v>16</v>
+      </c>
+      <c r="O18" s="10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
         <v>98029</v>
       </c>
       <c r="B19" t="s">
@@ -1647,9 +1789,15 @@
       <c r="M19" s="4">
         <v>1075</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="N19" s="10">
+        <v>36</v>
+      </c>
+      <c r="O19" s="10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <v>98030</v>
       </c>
       <c r="B20" s="4">
@@ -1688,9 +1836,15 @@
       <c r="M20">
         <v>867</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="N20" s="10">
+        <v>32</v>
+      </c>
+      <c r="O20" s="10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
         <v>98031</v>
       </c>
       <c r="B21" s="4">
@@ -1729,9 +1883,15 @@
       <c r="M21" s="4">
         <v>1457</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="N21" s="10">
+        <v>23</v>
+      </c>
+      <c r="O21" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
         <v>98032</v>
       </c>
       <c r="B22" s="4">
@@ -1770,9 +1930,15 @@
       <c r="M22" s="4">
         <v>1284</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="N22" s="10">
+        <v>17</v>
+      </c>
+      <c r="O22" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
         <v>98033</v>
       </c>
       <c r="B23" s="4">
@@ -1811,9 +1977,15 @@
       <c r="M23" s="4">
         <v>2054</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="N23" s="10">
+        <v>51</v>
+      </c>
+      <c r="O23" s="10">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
         <v>98034</v>
       </c>
       <c r="B24" s="4">
@@ -1852,9 +2024,15 @@
       <c r="M24" s="4">
         <v>1787</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="N24" s="10">
+        <v>26</v>
+      </c>
+      <c r="O24" s="10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
         <v>98038</v>
       </c>
       <c r="B25" s="4">
@@ -1893,9 +2071,15 @@
       <c r="M25" s="4">
         <v>1308</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="N25" s="10">
+        <v>42</v>
+      </c>
+      <c r="O25" s="10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
         <v>98039</v>
       </c>
       <c r="B26" t="s">
@@ -1934,9 +2118,15 @@
       <c r="M26">
         <v>379</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="N26" s="10">
+        <v>9</v>
+      </c>
+      <c r="O26" s="10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
         <v>98040</v>
       </c>
       <c r="B27" s="4">
@@ -1975,9 +2165,15 @@
       <c r="M27" s="4">
         <v>2168</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="N27" s="10">
+        <v>27</v>
+      </c>
+      <c r="O27" s="10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
         <v>98042</v>
       </c>
       <c r="B28" s="4">
@@ -2016,9 +2212,15 @@
       <c r="M28" s="4">
         <v>1995</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="N28" s="10">
+        <v>41</v>
+      </c>
+      <c r="O28" s="10">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
         <v>98045</v>
       </c>
       <c r="B29" t="s">
@@ -2057,9 +2259,15 @@
       <c r="M29">
         <v>622</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="N29" s="10">
+        <v>17</v>
+      </c>
+      <c r="O29" s="10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
         <v>98052</v>
       </c>
       <c r="B30" s="4">
@@ -2098,9 +2306,15 @@
       <c r="M30" s="4">
         <v>2666</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="N30" s="10">
+        <v>62</v>
+      </c>
+      <c r="O30" s="10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
         <v>98053</v>
       </c>
       <c r="B31" t="s">
@@ -2139,9 +2353,15 @@
       <c r="M31" s="4">
         <v>1191</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="N31" s="10">
+        <v>59</v>
+      </c>
+      <c r="O31" s="10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
         <v>98055</v>
       </c>
       <c r="B32" t="s">
@@ -2180,9 +2400,15 @@
       <c r="M32">
         <v>966</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="N32" s="10">
+        <v>18</v>
+      </c>
+      <c r="O32" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
         <v>98056</v>
       </c>
       <c r="B33" s="4">
@@ -2221,9 +2447,15 @@
       <c r="M33" s="4">
         <v>1410</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="N33" s="10">
+        <v>28</v>
+      </c>
+      <c r="O33" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
         <v>98058</v>
       </c>
       <c r="B34" s="4">
@@ -2262,9 +2494,15 @@
       <c r="M34" s="4">
         <v>2270</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="N34" s="10">
+        <v>35</v>
+      </c>
+      <c r="O34" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
         <v>98059</v>
       </c>
       <c r="B35" s="4">
@@ -2303,9 +2541,15 @@
       <c r="M35" s="4">
         <v>1945</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="N35" s="10">
+        <v>34</v>
+      </c>
+      <c r="O35" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
         <v>98065</v>
       </c>
       <c r="B36" s="4">
@@ -2344,9 +2588,15 @@
       <c r="M36">
         <v>323</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="N36" s="10">
+        <v>34</v>
+      </c>
+      <c r="O36" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
         <v>98070</v>
       </c>
       <c r="B37" s="4">
@@ -2385,9 +2635,15 @@
       <c r="M37" s="4">
         <v>1024</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="N37" s="10">
+        <v>12</v>
+      </c>
+      <c r="O37" s="10">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
         <v>98072</v>
       </c>
       <c r="B38" s="4">
@@ -2426,9 +2682,15 @@
       <c r="M38" s="4">
         <v>1189</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="N38" s="10">
+        <v>26</v>
+      </c>
+      <c r="O38" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
         <v>98074</v>
       </c>
       <c r="B39" s="4">
@@ -2467,9 +2729,15 @@
       <c r="M39">
         <v>924</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="N39" s="10">
+        <v>38</v>
+      </c>
+      <c r="O39" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
         <v>98075</v>
       </c>
       <c r="B40" s="4">
@@ -2508,9 +2776,15 @@
       <c r="M40">
         <v>783</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="N40" s="10">
+        <v>18</v>
+      </c>
+      <c r="O40" s="10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
         <v>98077</v>
       </c>
       <c r="B41" t="s">
@@ -2549,9 +2823,15 @@
       <c r="M41">
         <v>774</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="N41" s="10">
+        <v>12</v>
+      </c>
+      <c r="O41" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
         <v>98092</v>
       </c>
       <c r="B42" s="4">
@@ -2590,9 +2870,15 @@
       <c r="M42" s="4">
         <v>1894</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="N42" s="10">
+        <v>47</v>
+      </c>
+      <c r="O42" s="10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
         <v>98102</v>
       </c>
       <c r="B43" s="4">
@@ -2631,9 +2917,15 @@
       <c r="M43">
         <v>908</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="N43" s="10">
+        <v>34</v>
+      </c>
+      <c r="O43" s="10">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
         <v>98103</v>
       </c>
       <c r="B44" s="4">
@@ -2672,9 +2964,15 @@
       <c r="M44" s="4">
         <v>2194</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="N44" s="10">
+        <v>56</v>
+      </c>
+      <c r="O44" s="10">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
         <v>98105</v>
       </c>
       <c r="B45" s="4">
@@ -2713,9 +3011,15 @@
       <c r="M45" s="4">
         <v>1503</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="N45" s="10">
+        <v>60</v>
+      </c>
+      <c r="O45" s="10">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
         <v>98106</v>
       </c>
       <c r="B46" s="4">
@@ -2754,9 +3058,15 @@
       <c r="M46">
         <v>797</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="N46" s="10">
+        <v>30</v>
+      </c>
+      <c r="O46" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
         <v>98107</v>
       </c>
       <c r="B47" s="4">
@@ -2795,9 +3105,15 @@
       <c r="M47">
         <v>896</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="N47" s="10">
+        <v>25</v>
+      </c>
+      <c r="O47" s="10">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
         <v>98108</v>
       </c>
       <c r="B48" s="4">
@@ -2836,9 +3152,15 @@
       <c r="M48" s="4">
         <v>1194</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="N48" s="10">
+        <v>34</v>
+      </c>
+      <c r="O48" s="10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
         <v>98109</v>
       </c>
       <c r="B49" s="4">
@@ -2877,9 +3199,15 @@
       <c r="M49">
         <v>821</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="N49" s="10">
+        <v>54</v>
+      </c>
+      <c r="O49" s="10">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
         <v>98112</v>
       </c>
       <c r="B50" s="4">
@@ -2918,9 +3246,15 @@
       <c r="M50" s="4">
         <v>1543</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="N50" s="10">
+        <v>55</v>
+      </c>
+      <c r="O50" s="10">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
         <v>98115</v>
       </c>
       <c r="B51" s="4">
@@ -2959,9 +3293,15 @@
       <c r="M51" s="4">
         <v>3539</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="N51" s="10">
+        <v>71</v>
+      </c>
+      <c r="O51" s="10">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
         <v>98116</v>
       </c>
       <c r="B52" s="4">
@@ -3000,9 +3340,15 @@
       <c r="M52" s="4">
         <v>1496</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="N52" s="10">
+        <v>38</v>
+      </c>
+      <c r="O52" s="10">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
         <v>98117</v>
       </c>
       <c r="B53" s="4">
@@ -3041,9 +3387,15 @@
       <c r="M53" s="4">
         <v>2260</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="N53" s="10">
+        <v>45</v>
+      </c>
+      <c r="O53" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
         <v>98118</v>
       </c>
       <c r="B54" s="4">
@@ -3082,9 +3434,15 @@
       <c r="M54" s="4">
         <v>1797</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="N54" s="10">
+        <v>56</v>
+      </c>
+      <c r="O54" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
         <v>98119</v>
       </c>
       <c r="B55" s="4">
@@ -3123,9 +3481,15 @@
       <c r="M55">
         <v>989</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="N55" s="10">
+        <v>22</v>
+      </c>
+      <c r="O55" s="10">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
         <v>98122</v>
       </c>
       <c r="B56" s="4">
@@ -3164,9 +3528,15 @@
       <c r="M56">
         <v>867</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="N56" s="10">
+        <v>49</v>
+      </c>
+      <c r="O56" s="10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
         <v>98125</v>
       </c>
       <c r="B57" s="4">
@@ -3205,9 +3575,15 @@
       <c r="M57" s="4">
         <v>2099</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="N57" s="10">
+        <v>41</v>
+      </c>
+      <c r="O57" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
         <v>98126</v>
       </c>
       <c r="B58" s="4">
@@ -3246,9 +3622,15 @@
       <c r="M58">
         <v>989</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="N58" s="10">
+        <v>28</v>
+      </c>
+      <c r="O58" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
         <v>98133</v>
       </c>
       <c r="B59" s="4">
@@ -3287,9 +3669,15 @@
       <c r="M59" s="4">
         <v>2401</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="N59" s="10">
+        <v>32</v>
+      </c>
+      <c r="O59" s="10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
         <v>98136</v>
       </c>
       <c r="B60" t="s">
@@ -3328,9 +3716,15 @@
       <c r="M60" s="4">
         <v>1070</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="N60" s="10">
+        <v>19</v>
+      </c>
+      <c r="O60" s="10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
         <v>98144</v>
       </c>
       <c r="B61" s="4">
@@ -3369,9 +3763,15 @@
       <c r="M61" s="4">
         <v>1270</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="N61" s="10">
+        <v>46</v>
+      </c>
+      <c r="O61" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
         <v>98146</v>
       </c>
       <c r="B62" s="4">
@@ -3410,9 +3810,15 @@
       <c r="M62" s="4">
         <v>1495</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="N62" s="10">
+        <v>20</v>
+      </c>
+      <c r="O62" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A63" s="8">
         <v>98148</v>
       </c>
       <c r="B63" s="4">
@@ -3451,9 +3857,15 @@
       <c r="M63">
         <v>401</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="N63" s="10">
+        <v>4</v>
+      </c>
+      <c r="O63" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
         <v>98155</v>
       </c>
       <c r="B64" s="4">
@@ -3492,9 +3904,15 @@
       <c r="M64" s="4">
         <v>2173</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="N64" s="10">
+        <v>31</v>
+      </c>
+      <c r="O64" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A65" s="8">
         <v>98166</v>
       </c>
       <c r="B65" s="4">
@@ -3533,9 +3951,15 @@
       <c r="M65" s="4">
         <v>1624</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="N65" s="10">
+        <v>34</v>
+      </c>
+      <c r="O65" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
         <v>98168</v>
       </c>
       <c r="B66" t="s">
@@ -3574,9 +3998,15 @@
       <c r="M66" s="4">
         <v>1328</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="N66" s="10">
+        <v>30</v>
+      </c>
+      <c r="O66" s="10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A67" s="8">
         <v>98177</v>
       </c>
       <c r="B67" s="4">
@@ -3615,9 +4045,15 @@
       <c r="M67" s="4">
         <v>1846</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="N67" s="10">
+        <v>34</v>
+      </c>
+      <c r="O67" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
         <v>98178</v>
       </c>
       <c r="B68" s="4">
@@ -3656,9 +4092,15 @@
       <c r="M68" s="4">
         <v>1340</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="N68" s="10">
+        <v>33</v>
+      </c>
+      <c r="O68" s="10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A69" s="8">
         <v>98188</v>
       </c>
       <c r="B69" t="s">
@@ -3697,9 +4139,15 @@
       <c r="M69" s="4">
         <v>1335</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="N69" s="10">
+        <v>12</v>
+      </c>
+      <c r="O69" s="10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="A70" s="8">
         <v>98198</v>
       </c>
       <c r="B70" t="s">
@@ -3738,8 +4186,14 @@
       <c r="M70" s="4">
         <v>1799</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.25">
+      <c r="N70" s="10">
+        <v>29</v>
+      </c>
+      <c r="O70" s="10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>98199</v>
       </c>
@@ -3778,6 +4232,12 @@
       </c>
       <c r="M71" s="4">
         <v>1557</v>
+      </c>
+      <c r="N71" s="10">
+        <v>38</v>
+      </c>
+      <c r="O71" s="10">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>